<commit_message>
IG 14/08/23 handling LOD results, location map
</commit_message>
<xml_diff>
--- a/Data/WQ template example_data.xlsx
+++ b/Data/WQ template example_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apemltd365-my.sharepoint.com/personal/i_gordon_apemltd_co_uk/Documents/Documents/rProjects/WQ_analysis_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{6C76964A-8568-4100-BF1A-A7F967A77EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2079808-BEE8-4355-A7B4-31CFE11439F6}"/>
+  <xr:revisionPtr revIDLastSave="274" documentId="8_{6C76964A-8568-4100-BF1A-A7F967A77EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8DA091D-0C8F-4C5A-943A-3280F6E8AE23}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D24AB4D-DAA7-487D-B45C-1D6CEF40CC33}"/>
   </bookViews>
@@ -280,7 +280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="109">
   <si>
     <t>date_time</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>BOD ATU</t>
+  </si>
+  <si>
+    <t>&lt;0.01</t>
   </si>
 </sst>
 </file>
@@ -2595,7 +2598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2FF34F-184D-43F1-AA7D-07DA1F3A4C98}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2667,10 +2672,10 @@
         <v>100</v>
       </c>
       <c r="F2">
-        <v>101010</v>
+        <v>53.644744320000001</v>
       </c>
       <c r="G2">
-        <v>202020</v>
+        <v>-2.584067686</v>
       </c>
       <c r="H2">
         <v>9.4</v>
@@ -2708,10 +2713,10 @@
         <v>100</v>
       </c>
       <c r="F3">
-        <v>101010</v>
+        <v>53.644744320000001</v>
       </c>
       <c r="G3">
-        <v>202020</v>
+        <v>-2.584067686</v>
       </c>
       <c r="H3">
         <v>12.5</v>
@@ -2722,8 +2727,8 @@
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3">
-        <v>0.01</v>
+      <c r="K3" t="s">
+        <v>108</v>
       </c>
       <c r="L3">
         <v>0.53</v>
@@ -2749,10 +2754,10 @@
         <v>100</v>
       </c>
       <c r="F4">
-        <v>101010</v>
+        <v>53.644744320000001</v>
       </c>
       <c r="G4">
-        <v>202020</v>
+        <v>-2.584067686</v>
       </c>
       <c r="H4">
         <v>13.7</v>
@@ -2763,8 +2768,8 @@
       <c r="J4">
         <v>2.5</v>
       </c>
-      <c r="K4">
-        <v>0.01</v>
+      <c r="K4" t="s">
+        <v>108</v>
       </c>
       <c r="L4">
         <v>3.2000000000000001E-2</v>
@@ -2790,10 +2795,10 @@
         <v>100</v>
       </c>
       <c r="F5">
-        <v>101010</v>
+        <v>53.644744320000001</v>
       </c>
       <c r="G5">
-        <v>202020</v>
+        <v>-2.584067686</v>
       </c>
       <c r="H5">
         <v>7.5</v>
@@ -2804,8 +2809,8 @@
       <c r="J5">
         <v>2.6</v>
       </c>
-      <c r="K5">
-        <v>0.01</v>
+      <c r="K5" t="s">
+        <v>108</v>
       </c>
       <c r="L5">
         <v>7.0000000000000007E-2</v>
@@ -2831,10 +2836,10 @@
         <v>100</v>
       </c>
       <c r="F6">
-        <v>101010</v>
+        <v>53.644744320000001</v>
       </c>
       <c r="G6">
-        <v>202020</v>
+        <v>-2.584067686</v>
       </c>
       <c r="H6">
         <v>8.4</v>
@@ -2872,10 +2877,10 @@
         <v>101</v>
       </c>
       <c r="F7">
-        <v>202020</v>
+        <v>53.643474869999999</v>
       </c>
       <c r="G7">
-        <v>101010</v>
+        <v>-2.5834759630000002</v>
       </c>
       <c r="H7">
         <v>9.4</v>
@@ -2913,10 +2918,10 @@
         <v>101</v>
       </c>
       <c r="F8">
-        <v>202020</v>
+        <v>53.643474869999999</v>
       </c>
       <c r="G8">
-        <v>101010</v>
+        <v>-2.5834759630000002</v>
       </c>
       <c r="H8">
         <v>13</v>
@@ -2954,10 +2959,10 @@
         <v>101</v>
       </c>
       <c r="F9">
-        <v>202020</v>
+        <v>53.643474869999999</v>
       </c>
       <c r="G9">
-        <v>101010</v>
+        <v>-2.5834759630000002</v>
       </c>
       <c r="H9">
         <v>13.6</v>
@@ -2995,10 +3000,10 @@
         <v>101</v>
       </c>
       <c r="F10">
-        <v>202020</v>
+        <v>53.643474869999999</v>
       </c>
       <c r="G10">
-        <v>101010</v>
+        <v>-2.5834759630000002</v>
       </c>
       <c r="H10">
         <v>7.4</v>
@@ -3036,10 +3041,10 @@
         <v>101</v>
       </c>
       <c r="F11">
-        <v>202020</v>
+        <v>53.643474869999999</v>
       </c>
       <c r="G11">
-        <v>101010</v>
+        <v>-2.5834759630000002</v>
       </c>
       <c r="H11">
         <v>7.5</v>

</xml_diff>

<commit_message>
IG 19/10/23 nesting facets to identify us/ds WBs
</commit_message>
<xml_diff>
--- a/Data/WQ template example_data.xlsx
+++ b/Data/WQ template example_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apemltd365-my.sharepoint.com/personal/i_gordon_apemltd_co_uk/Documents/Documents/rProjects/WQ_analysis_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F45E377B-A3CD-4106-80E8-B719AD83088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBC5D330-E93C-41EC-8D3B-BA0C6814E7DC}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{F45E377B-A3CD-4106-80E8-B719AD83088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50019987-CC83-4236-8399-5786E655DFB8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D24AB4D-DAA7-487D-B45C-1D6CEF40CC33}"/>
   </bookViews>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="138">
   <si>
     <t>date_time</t>
   </si>
@@ -683,6 +683,18 @@
   </si>
   <si>
     <t>tributary</t>
+  </si>
+  <si>
+    <t>WQ15</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>Upstream</t>
+  </si>
+  <si>
+    <t>Downstream</t>
   </si>
 </sst>
 </file>
@@ -690,7 +702,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1215,7 +1227,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1232,8 +1244,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1279,7 +1290,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1741,7 +1759,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD23E511-5561-49DD-8572-41AF4730906A}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1844,7 +1864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42615C5C-FF4C-4E67-B33A-525073A52AEF}">
   <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2101,7 +2123,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>45096.475949074076</v>
       </c>
       <c r="B7" t="s">
@@ -2142,7 +2164,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>45096.476087962961</v>
       </c>
       <c r="B8" t="s">
@@ -2183,7 +2205,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>45096.47625</v>
       </c>
       <c r="B9" t="s">
@@ -2224,7 +2246,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>45096.476527777777</v>
       </c>
       <c r="B10" t="s">
@@ -2265,7 +2287,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>45096.476666666669</v>
       </c>
       <c r="B11" t="s">
@@ -2306,7 +2328,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>45096.4768287037</v>
       </c>
       <c r="B12" t="s">
@@ -2347,63 +2369,253 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="10">
+        <v>45096.469837962963</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13">
+        <v>53.644744320000001</v>
+      </c>
+      <c r="D13">
+        <v>-2.584067686</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>20.313300000000002</v>
+      </c>
+      <c r="G13">
+        <v>92.777320000000003</v>
+      </c>
+      <c r="H13">
+        <v>8.2005809999999997</v>
+      </c>
+      <c r="I13">
+        <v>7.3812949999999997</v>
+      </c>
+      <c r="J13">
+        <v>0.14054230000000001</v>
+      </c>
+      <c r="K13">
+        <v>82.292479999999998</v>
+      </c>
+      <c r="L13">
+        <v>90.346860000000007</v>
+      </c>
+      <c r="M13">
+        <v>4.2111009999999997E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="10">
+        <v>45096.470324074071</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14">
+        <v>53.644755189999998</v>
+      </c>
+      <c r="D14">
+        <v>-2.584081442</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>20.365469999999998</v>
+      </c>
+      <c r="G14">
+        <v>92.598879999999994</v>
+      </c>
+      <c r="H14">
+        <v>8.1805280000000007</v>
+      </c>
+      <c r="I14">
+        <v>7.3252730000000001</v>
+      </c>
+      <c r="J14">
+        <v>0.56833540000000005</v>
+      </c>
+      <c r="K14">
+        <v>83.586429999999993</v>
+      </c>
+      <c r="L14">
+        <v>91.70402</v>
+      </c>
+      <c r="M14">
+        <v>4.2769729999999999E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="10">
+        <v>45096.470648148148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15">
+        <v>53.644750469999998</v>
+      </c>
+      <c r="D15">
+        <v>-2.5840798330000001</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15">
+        <v>20.353649999999998</v>
+      </c>
+      <c r="G15">
+        <v>92.491500000000002</v>
+      </c>
+      <c r="H15">
+        <v>8.1733080000000005</v>
+      </c>
+      <c r="I15">
+        <v>7.3290550000000003</v>
+      </c>
+      <c r="J15">
+        <v>1.0747359999999999</v>
+      </c>
+      <c r="K15">
+        <v>83.512979999999999</v>
+      </c>
+      <c r="L15">
+        <v>91.646150000000006</v>
+      </c>
+      <c r="M15">
+        <v>4.2741590000000003E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>45096.470810185187</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16">
+        <v>53.644743890000001</v>
+      </c>
+      <c r="D16">
+        <v>-2.584077948</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16">
+        <v>20.359290000000001</v>
+      </c>
+      <c r="G16">
+        <v>92.513729999999995</v>
+      </c>
+      <c r="H16">
+        <v>8.1747610000000002</v>
+      </c>
+      <c r="I16">
+        <v>7.3224749999999998</v>
+      </c>
+      <c r="J16">
+        <v>1.5130429999999999</v>
+      </c>
+      <c r="K16">
+        <v>83.549520000000001</v>
+      </c>
+      <c r="L16">
+        <v>91.675409999999999</v>
+      </c>
+      <c r="M16">
+        <v>4.275582E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>45096.475138888891</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17">
+        <v>53.643476870000001</v>
+      </c>
+      <c r="D17">
+        <v>-2.5834600719999998</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17">
+        <v>20.33174</v>
+      </c>
+      <c r="G17">
+        <v>89.359889999999993</v>
+      </c>
+      <c r="H17">
+        <v>7.8993659999999997</v>
+      </c>
+      <c r="I17">
+        <v>7.2339019999999996</v>
+      </c>
+      <c r="J17">
+        <v>0.1532975</v>
+      </c>
+      <c r="K17">
+        <v>83.18571</v>
+      </c>
+      <c r="L17">
+        <v>91.328950000000006</v>
+      </c>
+      <c r="M17">
+        <v>4.2587590000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
@@ -2626,20 +2838,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{95AC579E-BD6D-4B62-B453-1AACABCBE620}">
-            <xm:f>AND(NOT(B13=""),OR(ISERROR(MATCH(B13, MANUAL_FIELD!$D:$D,0)), ISERROR(MATCH(B13, LAB_DATA!$E:$E,0))))</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B13:B500</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{CDCC9EB2-7D73-43F9-BE14-CBB2C376A345}">
+          <x14:cfRule type="expression" priority="3" id="{CDCC9EB2-7D73-43F9-BE14-CBB2C376A345}">
             <xm:f>AND(NOT(A2=""),OR(ISERROR(MATCH(B2, $B:$B,0)), ISERROR(MATCH(B2,MANUAL_FIELD!$D:$D,0))))</xm:f>
             <x14:dxf>
               <fill>
@@ -2652,7 +2851,7 @@
           <xm:sqref>B2:B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{1A6F5130-FA3C-415A-AD1D-58FACF84B143}">
+          <x14:cfRule type="expression" priority="2" id="{1A6F5130-FA3C-415A-AD1D-58FACF84B143}">
             <xm:f>AND(NOT(B7=""),OR(ISERROR(MATCH(B7, $B:$B,0)), ISERROR(MATCH(B7, LAB_DATA!$E:$E,0))))</xm:f>
             <x14:dxf>
               <fill>
@@ -2663,6 +2862,32 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>B7:B12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{E322D9AD-0DB6-4F38-B5F2-D5CE43B84FCB}">
+            <xm:f>AND(NOT(A13=""),OR(ISERROR(MATCH(B13, $B:$B,0)), ISERROR(MATCH(B13,MANUAL_FIELD!$D:$D,0))))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B13:B17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{95AC579E-BD6D-4B62-B453-1AACABCBE620}">
+            <xm:f>AND(NOT(B18=""),OR(ISERROR(MATCH(B18, MANUAL_FIELD!$D:$D,0)), ISERROR(MATCH(B18, LAB_DATA!$E:$E,0))))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B18:B500</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3683,13 +3908,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE21C24D-AA85-4B97-B134-5D4640E26252}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3708,10 +3933,13 @@
       <c r="F1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A3">IF(PROBE_DATA!B2&lt;&gt;"", _xlfn.UNIQUE(_xlfn._xlws.FILTER(PROBE_DATA!B2:B1000,PROBE_DATA!B2:B1000&lt;&gt;"")), IF(MANUAL_FIELD!D2 &lt;&gt; "", _xlfn.UNIQUE(_xlfn._xlws.FILTER(MANUAL_FIELD!D2:D1000,MANUAL_FIELD!D2:D1000&lt;&gt;"")), IF(LAB_DATA!E2 &lt;&gt; "", _xlfn.UNIQUE(_xlfn._xlws.FILTER(LAB_DATA!E2:E1000,LAB_DATA!E2:E1000&lt;&gt;"")))))</f>
+        <f t="array" ref="A2:A4">IF(PROBE_DATA!B2&lt;&gt;"", _xlfn.UNIQUE(_xlfn._xlws.FILTER(PROBE_DATA!B2:B1000,PROBE_DATA!B2:B1000&lt;&gt;"")), IF(MANUAL_FIELD!D2 &lt;&gt; "", _xlfn.UNIQUE(_xlfn._xlws.FILTER(MANUAL_FIELD!D2:D1000,MANUAL_FIELD!D2:D1000&lt;&gt;"")), IF(LAB_DATA!E2 &lt;&gt; "", _xlfn.UNIQUE(_xlfn._xlws.FILTER(LAB_DATA!E2:E1000,LAB_DATA!E2:E1000&lt;&gt;"")))))</f>
         <v>WQ13</v>
       </c>
       <c r="B2">
@@ -3730,8 +3958,11 @@
       <c r="F2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <v>WQ14</v>
       </c>
@@ -3751,80 +3982,97 @@
       <c r="F3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="str">
-        <f>IF(A4&lt;&gt;"",IFERROR(VLOOKUP(A4,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A4,LAB_DATA!E:F,2,FALSE),"")), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <v>WQ15</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="str">
         <f>IF(A5&lt;&gt;"",IFERROR(VLOOKUP(A5,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A5,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" t="str">
         <f>IF(A6&lt;&gt;"",IFERROR(VLOOKUP(A6,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A6,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f>IF(A7&lt;&gt;"",IFERROR(VLOOKUP(A7,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A7,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <f>IF(A8&lt;&gt;"",IFERROR(VLOOKUP(A8,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A8,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f>IF(A9&lt;&gt;"",IFERROR(VLOOKUP(A9,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A9,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
         <f>IF(A10&lt;&gt;"",IFERROR(VLOOKUP(A10,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A10,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f>IF(A11&lt;&gt;"",IFERROR(VLOOKUP(A11,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A11,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>IF(A12&lt;&gt;"",IFERROR(VLOOKUP(A12,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A12,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>IF(A13&lt;&gt;"",IFERROR(VLOOKUP(A13,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A13,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <f>IF(A14&lt;&gt;"",IFERROR(VLOOKUP(A14,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A14,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <f>IF(A15&lt;&gt;"",IFERROR(VLOOKUP(A15,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A15,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="str">
         <f>IF(A16&lt;&gt;"",IFERROR(VLOOKUP(A16,MANUAL_FIELD!D:E,2,FALSE),IFERROR(VLOOKUP(A16,LAB_DATA!E:F,2,FALSE),"")), "")</f>
         <v/>
@@ -3855,13 +4103,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{59927F3F-EB58-49E7-850B-689B398F348A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{59927F3F-EB58-49E7-850B-689B398F348A}">
       <formula1>"Salmonid, Cyprinid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{33AFB69B-7F05-4D5D-87E6-5ADE6217E122}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{33AFB69B-7F05-4D5D-87E6-5ADE6217E122}">
       <formula1>"Upland, Lowland"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{0C41E39A-A4B2-4C77-B243-A5F903D9D6BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{0C41E39A-A4B2-4C77-B243-A5F903D9D6BB}">
       <formula1>"main, tributary"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>